<commit_message>
Pull in schedule from spreadsheet - see https://github.com/STAT545-UBC/STAT545-UBC.github.io/blob/master/syllabus.Rmd
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -29,81 +29,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
-    <t>module</t>
-  </si>
-  <si>
     <t>topic</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>005</t>
-  </si>
-  <si>
-    <t>006</t>
-  </si>
-  <si>
-    <t>007</t>
-  </si>
-  <si>
-    <t>008</t>
-  </si>
-  <si>
-    <t>009</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>011</t>
-  </si>
-  <si>
-    <t>012</t>
-  </si>
-  <si>
-    <t>013</t>
-  </si>
-  <si>
-    <t>014</t>
-  </si>
-  <si>
-    <t>015</t>
-  </si>
-  <si>
-    <t>016</t>
-  </si>
-  <si>
-    <t>017</t>
-  </si>
-  <si>
-    <t>018</t>
-  </si>
-  <si>
-    <t>019</t>
-  </si>
-  <si>
-    <t>020</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
-    <t>Introduction to computational social science, basic principles of programming, and the programming language Python</t>
-  </si>
-  <si>
-    <t>Introduction to control flow. Introduction to functions.</t>
-  </si>
-  <si>
     <t>Functions (cont.)</t>
   </si>
   <si>
@@ -149,9 +80,6 @@
     <t>Interactivity</t>
   </si>
   <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>Shiny objects</t>
   </si>
   <si>
@@ -159,6 +87,78 @@
   </si>
   <si>
     <t>Parallelization</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>cm001</t>
+  </si>
+  <si>
+    <t>cm002</t>
+  </si>
+  <si>
+    <t>cm003</t>
+  </si>
+  <si>
+    <t>cm004</t>
+  </si>
+  <si>
+    <t>cm005</t>
+  </si>
+  <si>
+    <t>cm006</t>
+  </si>
+  <si>
+    <t>cm007</t>
+  </si>
+  <si>
+    <t>cm008</t>
+  </si>
+  <si>
+    <t>cm009</t>
+  </si>
+  <si>
+    <t>cm010</t>
+  </si>
+  <si>
+    <t>cm011</t>
+  </si>
+  <si>
+    <t>cm012</t>
+  </si>
+  <si>
+    <t>cm013</t>
+  </si>
+  <si>
+    <t>cm014</t>
+  </si>
+  <si>
+    <t>cm015</t>
+  </si>
+  <si>
+    <t>cm016</t>
+  </si>
+  <si>
+    <t>cm017</t>
+  </si>
+  <si>
+    <t>cm018</t>
+  </si>
+  <si>
+    <t>cm019</t>
+  </si>
+  <si>
+    <t>cm020</t>
+  </si>
+  <si>
+    <t>link_it</t>
+  </si>
+  <si>
+    <t>Introduction to computational social science, basic principles of programming, and Python</t>
+  </si>
+  <si>
+    <t>Loops, conditionals, and functions</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection sqref="A1:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,21 +489,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2">
         <v>42639</v>
@@ -512,12 +512,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
@@ -527,12 +527,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
@@ -542,27 +542,27 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ref="B5:B21" si="0">B4+2</f>
+        <f t="shared" ref="B5" si="0">B4+2</f>
         <v>42648</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
@@ -572,27 +572,27 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" ref="B7:B21" si="2">B6+2</f>
+        <f t="shared" ref="B7" si="2">B6+2</f>
         <v>42655</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
@@ -602,27 +602,27 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" ref="B9:B21" si="4">B8+2</f>
+        <f t="shared" ref="B9" si="4">B8+2</f>
         <v>42662</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
@@ -632,27 +632,27 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" ref="B11:B21" si="6">B10+2</f>
+        <f t="shared" ref="B11" si="6">B10+2</f>
         <v>42669</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
@@ -662,27 +662,27 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" ref="B13:B21" si="8">B12+2</f>
+        <f t="shared" ref="B13" si="8">B12+2</f>
         <v>42676</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
@@ -692,27 +692,27 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" ref="B15:B21" si="10">B14+2</f>
+        <f t="shared" ref="B15" si="10">B14+2</f>
         <v>42683</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
@@ -722,27 +722,27 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" ref="B17:B21" si="12">B16+2</f>
+        <f t="shared" ref="B17" si="12">B16+2</f>
         <v>42690</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
@@ -752,27 +752,27 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ref="B19:B21" si="14">B18+2</f>
+        <f t="shared" ref="B19" si="14">B18+2</f>
         <v>42697</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
@@ -782,12 +782,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the schedule to add data pipelines
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -50,12 +50,6 @@
     <t>Data wrangling</t>
   </si>
   <si>
-    <t>Programming in R - piping and functions</t>
-  </si>
-  <si>
-    <t>Programming in R - vectors, iteration</t>
-  </si>
-  <si>
     <t>Models in R</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>Loops, conditionals, and functions</t>
+  </si>
+  <si>
+    <t>Programming in R</t>
+  </si>
+  <si>
+    <t>Data pipelines</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:D21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,13 +489,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -503,7 +503,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2">
         <v>42639</v>
@@ -512,12 +512,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
@@ -527,12 +527,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
@@ -547,7 +547,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
@@ -562,7 +562,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
@@ -577,7 +577,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
@@ -592,7 +592,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
@@ -607,7 +607,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
@@ -617,12 +617,12 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
@@ -632,12 +632,12 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
@@ -647,12 +647,12 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
@@ -662,12 +662,12 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
@@ -677,12 +677,12 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
@@ -692,12 +692,12 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
@@ -707,12 +707,12 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
@@ -722,12 +722,12 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
@@ -737,12 +737,12 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
@@ -752,12 +752,12 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
@@ -767,12 +767,12 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
@@ -782,12 +782,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Rstudio -> RStudio
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/techbar/macss-programming/course_admin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/techbar/MACS-30500/course_admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,9 +41,6 @@
     <t>Code style, efficiency, and debugging</t>
   </si>
   <si>
-    <t>Introduction to R, Rstudio, and the tidyverse</t>
-  </si>
-  <si>
     <t>Data visualization</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Data pipelines</t>
+  </si>
+  <si>
+    <t>Introduction to R, RStudio, and the tidyverse</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,13 +489,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -503,7 +503,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2">
         <v>42639</v>
@@ -512,12 +512,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
@@ -527,12 +527,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
@@ -547,7 +547,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
@@ -562,7 +562,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
@@ -572,12 +572,12 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
@@ -587,12 +587,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
@@ -602,12 +602,12 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
@@ -617,12 +617,12 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
@@ -632,12 +632,12 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
@@ -647,12 +647,12 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
@@ -662,12 +662,12 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
@@ -677,12 +677,12 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
@@ -692,12 +692,12 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
@@ -707,12 +707,12 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
@@ -722,12 +722,12 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
@@ -737,12 +737,12 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
@@ -752,12 +752,12 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
@@ -767,12 +767,12 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
@@ -782,12 +782,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update schedule topic title
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/techbar/MACS-30500/course_admin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Computing for Social Sciences/uc-cfss.github.io/course_admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,9 +16,6 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -155,10 +152,10 @@
     <t>Programming in R</t>
   </si>
   <si>
-    <t>Data pipelines</t>
-  </si>
-  <si>
     <t>Introduction to R, RStudio, and the tidyverse</t>
+  </si>
+  <si>
+    <t>Data pipelines and reproducibility</t>
   </si>
 </sst>
 </file>
@@ -478,7 +475,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,7 +569,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -647,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Minor edits to setup instructions
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -475,7 +478,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,7 +509,7 @@
         <v>42639</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Add software installation to syllabus
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>topic</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>Data pipelines and reproducibility</t>
+  </si>
+  <si>
+    <t>setup00</t>
+  </si>
+  <si>
+    <t>Software installation</t>
   </si>
 </sst>
 </file>
@@ -475,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,300 +509,311 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2">
-        <v>42639</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2">
-        <f>B2+2</f>
-        <v>42641</v>
+        <v>42639</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2">
-        <f>B2+7</f>
-        <v>42646</v>
+        <f>B3+2</f>
+        <v>42641</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ref="B5" si="0">B4+2</f>
-        <v>42648</v>
+        <f>B3+7</f>
+        <v>42646</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ref="B6" si="1">B4+7</f>
-        <v>42653</v>
+        <f t="shared" ref="B6" si="0">B5+2</f>
+        <v>42648</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" ref="B7" si="2">B6+2</f>
-        <v>42655</v>
+        <f t="shared" ref="B7" si="1">B5+7</f>
+        <v>42653</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" ref="B8" si="3">B6+7</f>
-        <v>42660</v>
+        <f t="shared" ref="B8" si="2">B7+2</f>
+        <v>42655</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" ref="B9" si="4">B8+2</f>
-        <v>42662</v>
+        <f t="shared" ref="B9" si="3">B7+7</f>
+        <v>42660</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" ref="B10" si="5">B8+7</f>
-        <v>42667</v>
+        <f t="shared" ref="B10" si="4">B9+2</f>
+        <v>42662</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" ref="B11" si="6">B10+2</f>
-        <v>42669</v>
+        <f t="shared" ref="B11" si="5">B9+7</f>
+        <v>42667</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2">
-        <f t="shared" ref="B12" si="7">B10+7</f>
-        <v>42674</v>
+        <f t="shared" ref="B12" si="6">B11+2</f>
+        <v>42669</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" ref="B13" si="8">B12+2</f>
-        <v>42676</v>
+        <f t="shared" ref="B13" si="7">B11+7</f>
+        <v>42674</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2">
-        <f t="shared" ref="B14" si="9">B12+7</f>
-        <v>42681</v>
+        <f t="shared" ref="B14" si="8">B13+2</f>
+        <v>42676</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" ref="B15" si="10">B14+2</f>
-        <v>42683</v>
+        <f t="shared" ref="B15" si="9">B13+7</f>
+        <v>42681</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" ref="B16" si="11">B14+7</f>
-        <v>42688</v>
+        <f t="shared" ref="B16" si="10">B15+2</f>
+        <v>42683</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" ref="B17" si="12">B16+2</f>
-        <v>42690</v>
+        <f t="shared" ref="B17" si="11">B15+7</f>
+        <v>42688</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2">
-        <f t="shared" ref="B18" si="13">B16+7</f>
-        <v>42695</v>
+        <f t="shared" ref="B18" si="12">B17+2</f>
+        <v>42690</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ref="B19" si="14">B18+2</f>
-        <v>42697</v>
+        <f t="shared" ref="B19" si="13">B17+7</f>
+        <v>42695</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" ref="B20" si="15">B18+7</f>
-        <v>42702</v>
+        <f t="shared" ref="B20" si="14">B19+2</f>
+        <v>42697</v>
       </c>
       <c r="C20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" ref="B21" si="15">B19+7</f>
+        <v>42702</v>
+      </c>
+      <c r="C21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="2">
-        <f t="shared" ref="B21" si="16">B20+2</f>
+      <c r="B22" s="2">
+        <f t="shared" ref="B22" si="16">B21+2</f>
         <v>42704</v>
       </c>
-      <c r="C21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update schedule to emphasize R in initial weeks
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16240" yWindow="460" windowWidth="12560" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="16240" yWindow="460" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>topic</t>
   </si>
@@ -35,12 +35,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>Functions (cont.)</t>
-  </si>
-  <si>
-    <t>Code style, efficiency, and debugging</t>
-  </si>
-  <si>
     <t>Data visualization</t>
   </si>
   <si>
@@ -146,25 +140,28 @@
     <t>link_it</t>
   </si>
   <si>
-    <t>Introduction to computational social science, basic principles of programming, and Python</t>
-  </si>
-  <si>
-    <t>Loops, conditionals, and functions</t>
-  </si>
-  <si>
     <t>Programming in R</t>
   </si>
   <si>
-    <t>Introduction to R, RStudio, and the tidyverse</t>
-  </si>
-  <si>
-    <t>Data pipelines and reproducibility</t>
-  </si>
-  <si>
     <t>setup00</t>
   </si>
   <si>
     <t>Software installation</t>
+  </si>
+  <si>
+    <t>Introduction to computational social science, R, git, and workflow</t>
+  </si>
+  <si>
+    <t>Exploratory data analysis</t>
+  </si>
+  <si>
+    <t>Introduction to Python</t>
+  </si>
+  <si>
+    <t>Functional programming in Python</t>
+  </si>
+  <si>
+    <t>Data pipelines, communication, and reproducibility</t>
   </si>
 </sst>
 </file>
@@ -484,7 +481,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,13 +492,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -509,18 +506,18 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2">
         <v>42639</v>
@@ -529,12 +526,12 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2">
         <f>B3+2</f>
@@ -544,12 +541,12 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2">
         <f>B3+7</f>
@@ -559,12 +556,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="0">B5+2</f>
@@ -579,7 +576,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="1">B5+7</f>
@@ -589,12 +586,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="2">B7+2</f>
@@ -604,12 +601,12 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="3">B7+7</f>
@@ -619,12 +616,12 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="4">B9+2</f>
@@ -634,12 +631,12 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="5">B9+7</f>
@@ -649,12 +646,12 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="6">B11+2</f>
@@ -664,12 +661,12 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="7">B11+7</f>
@@ -679,12 +676,12 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="8">B13+2</f>
@@ -694,12 +691,12 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="9">B13+7</f>
@@ -709,12 +706,12 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="10">B15+2</f>
@@ -724,12 +721,12 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="11">B15+7</f>
@@ -739,12 +736,12 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="12">B17+2</f>
@@ -754,12 +751,12 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="13">B17+7</f>
@@ -769,12 +766,12 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="14">B19+2</f>
@@ -784,12 +781,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="15">B19+7</f>
@@ -799,12 +796,12 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" ref="B22" si="16">B21+2</f>
@@ -814,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust topic schedule to move API access next to web scraping
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16240" yWindow="460" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="7560" yWindow="460" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Models in R</t>
   </si>
   <si>
-    <t>Web scraping</t>
-  </si>
-  <si>
     <t>Network analysis</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Data warehousing and relational databases</t>
   </si>
   <si>
-    <t>API access</t>
-  </si>
-  <si>
     <t>Interactivity</t>
   </si>
   <si>
@@ -162,6 +156,12 @@
   </si>
   <si>
     <t>Introduction to computing for the social sciences</t>
+  </si>
+  <si>
+    <t>Getting data from the web: API access</t>
+  </si>
+  <si>
+    <t>Getting data from the web: scraping</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,13 +492,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -506,18 +506,18 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2">
         <v>42639</v>
@@ -526,12 +526,12 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2">
         <f>B3+2</f>
@@ -546,7 +546,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2">
         <f>B3+7</f>
@@ -556,12 +556,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="0">B5+2</f>
@@ -576,7 +576,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="1">B5+7</f>
@@ -586,12 +586,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="2">B7+2</f>
@@ -601,12 +601,12 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="3">B7+7</f>
@@ -621,7 +621,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="4">B9+2</f>
@@ -636,7 +636,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="5">B9+7</f>
@@ -646,12 +646,12 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="6">B11+2</f>
@@ -661,12 +661,12 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="7">B11+7</f>
@@ -676,12 +676,12 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="8">B13+2</f>
@@ -691,12 +691,12 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="9">B13+7</f>
@@ -706,12 +706,12 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="10">B15+2</f>
@@ -721,12 +721,12 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="11">B15+7</f>
@@ -736,12 +736,12 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="12">B17+2</f>
@@ -751,12 +751,12 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="13">B17+7</f>
@@ -766,12 +766,12 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="14">B19+2</f>
@@ -781,12 +781,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="15">B19+7</f>
@@ -796,12 +796,12 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" ref="B22" si="16">B21+2</f>
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update syllabus for cm002
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -155,13 +155,13 @@
     <t>Getting data from the web: scraping</t>
   </si>
   <si>
-    <t>Programming, version control software, &amp; grammar of graphics</t>
-  </si>
-  <si>
     <t>Data pipelines, the shell, communication, and reproducibility</t>
   </si>
   <si>
     <t>Simulation</t>
+  </si>
+  <si>
+    <t>Grammar of graphics and version control software</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add lab sessions to syllabus
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>topic</t>
   </si>
@@ -162,6 +162,54 @@
   </si>
   <si>
     <t>Grammar of graphics and version control software</t>
+  </si>
+  <si>
+    <t>Software setup</t>
+  </si>
+  <si>
+    <t>Advanced programming tips</t>
+  </si>
+  <si>
+    <t>The shell</t>
+  </si>
+  <si>
+    <t>Pandas</t>
+  </si>
+  <si>
+    <t>RMarkdown websites</t>
+  </si>
+  <si>
+    <t>lab01</t>
+  </si>
+  <si>
+    <t>lab02</t>
+  </si>
+  <si>
+    <t>lab03</t>
+  </si>
+  <si>
+    <t>lab04</t>
+  </si>
+  <si>
+    <t>lab05</t>
+  </si>
+  <si>
+    <t>lab06</t>
+  </si>
+  <si>
+    <t>lab07</t>
+  </si>
+  <si>
+    <t>lab08</t>
+  </si>
+  <si>
+    <t>lab09</t>
+  </si>
+  <si>
+    <t>lab10</t>
+  </si>
+  <si>
+    <t>RMarkdown</t>
   </si>
 </sst>
 </file>
@@ -478,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,6 +862,143 @@
         <v>9</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="2">
+        <v>42641</v>
+      </c>
+      <c r="C23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="2">
+        <f>B23+7</f>
+        <v>42648</v>
+      </c>
+      <c r="C24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" ref="B25:B32" si="17">B24+7</f>
+        <v>42655</v>
+      </c>
+      <c r="C25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="17"/>
+        <v>42662</v>
+      </c>
+      <c r="C26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="17"/>
+        <v>42669</v>
+      </c>
+      <c r="C27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="17"/>
+        <v>42676</v>
+      </c>
+      <c r="C28" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2">
+        <f t="shared" si="17"/>
+        <v>42683</v>
+      </c>
+      <c r="C29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="2">
+        <f t="shared" si="17"/>
+        <v>42690</v>
+      </c>
+      <c r="C30" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="2">
+        <f t="shared" si="17"/>
+        <v>42697</v>
+      </c>
+      <c r="C31" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="2">
+        <f t="shared" si="17"/>
+        <v>42704</v>
+      </c>
+      <c r="C32" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rewrite `syllabus.Rmd` to make more efficient
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>topic</t>
   </si>
@@ -129,12 +129,6 @@
   </si>
   <si>
     <t>Programming in R</t>
-  </si>
-  <si>
-    <t>setup00</t>
-  </si>
-  <si>
-    <t>Software installation</t>
   </si>
   <si>
     <t>Exploratory data analysis</t>
@@ -526,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,81 +548,85 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
+        <v>42639</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>42639</v>
+        <f>B2+2</f>
+        <v>42641</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
-        <f>B3+2</f>
-        <v>42641</v>
+        <f>B2+7</f>
+        <v>42646</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
-        <f>B3+7</f>
-        <v>42646</v>
+        <f t="shared" ref="B5" si="0">B4+2</f>
+        <v>42648</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ref="B6" si="0">B5+2</f>
-        <v>42648</v>
+        <f t="shared" ref="B6" si="1">B4+7</f>
+        <v>42653</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" ref="B7" si="1">B5+7</f>
-        <v>42653</v>
+        <f t="shared" ref="B7" si="2">B6+2</f>
+        <v>42655</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -639,71 +637,71 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" ref="B8" si="2">B7+2</f>
-        <v>42655</v>
+        <f t="shared" ref="B8" si="3">B6+7</f>
+        <v>42660</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" ref="B9" si="3">B7+7</f>
-        <v>42660</v>
+        <f t="shared" ref="B9" si="4">B8+2</f>
+        <v>42662</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" ref="B10" si="4">B9+2</f>
-        <v>42662</v>
+        <f t="shared" ref="B10" si="5">B8+7</f>
+        <v>42667</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" ref="B11" si="5">B9+7</f>
-        <v>42667</v>
+        <f t="shared" ref="B11" si="6">B10+2</f>
+        <v>42669</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2">
-        <f t="shared" ref="B12" si="6">B11+2</f>
-        <v>42669</v>
+        <f t="shared" ref="B12" si="7">B10+7</f>
+        <v>42674</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>0</v>
@@ -714,262 +712,259 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" ref="B13" si="7">B11+7</f>
-        <v>42674</v>
+        <f t="shared" ref="B13" si="8">B12+2</f>
+        <v>42676</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2">
-        <f t="shared" ref="B14" si="8">B13+2</f>
-        <v>42676</v>
+        <f t="shared" ref="B14" si="9">B12+7</f>
+        <v>42681</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" ref="B15" si="9">B13+7</f>
-        <v>42681</v>
+        <f t="shared" ref="B15" si="10">B14+2</f>
+        <v>42683</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" ref="B16" si="10">B15+2</f>
-        <v>42683</v>
+        <f t="shared" ref="B16" si="11">B14+7</f>
+        <v>42688</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" ref="B17" si="11">B15+7</f>
-        <v>42688</v>
+        <f t="shared" ref="B17" si="12">B16+2</f>
+        <v>42690</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2">
-        <f t="shared" ref="B18" si="12">B17+2</f>
-        <v>42690</v>
+        <f t="shared" ref="B18" si="13">B16+7</f>
+        <v>42695</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ref="B19" si="13">B17+7</f>
-        <v>42695</v>
+        <f t="shared" ref="B19" si="14">B18+2</f>
+        <v>42697</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" ref="B20" si="14">B19+2</f>
-        <v>42697</v>
+        <f t="shared" ref="B20" si="15">B18+7</f>
+        <v>42702</v>
       </c>
       <c r="C20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" ref="B21" si="15">B19+7</f>
-        <v>42702</v>
+        <f t="shared" ref="B21" si="16">B20+2</f>
+        <v>42704</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B22" s="2">
-        <f t="shared" ref="B22" si="16">B21+2</f>
-        <v>42704</v>
+        <v>42641</v>
       </c>
       <c r="C22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2">
-        <v>42641</v>
+        <f>B22+7</f>
+        <v>42648</v>
       </c>
       <c r="C23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2">
-        <f>B23+7</f>
-        <v>42648</v>
+        <f t="shared" ref="B24:B31" si="17">B23+7</f>
+        <v>42655</v>
       </c>
       <c r="C24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" ref="B25:B32" si="17">B24+7</f>
-        <v>42655</v>
+        <f t="shared" si="17"/>
+        <v>42662</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="17"/>
-        <v>42662</v>
+        <v>42669</v>
       </c>
       <c r="C26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="17"/>
-        <v>42669</v>
+        <v>42676</v>
       </c>
       <c r="C27" s="2" t="b">
         <v>0</v>
-      </c>
-      <c r="D27" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="17"/>
-        <v>42676</v>
+        <v>42683</v>
       </c>
       <c r="C28" s="2" t="b">
         <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="17"/>
-        <v>42683</v>
+        <v>42690</v>
       </c>
       <c r="C29" s="2" t="b">
         <v>0</v>
-      </c>
-      <c r="D29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="17"/>
-        <v>42690</v>
+        <v>42697</v>
       </c>
       <c r="C30" s="2" t="b">
         <v>0</v>
@@ -977,25 +972,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="17"/>
-        <v>42697</v>
+        <v>42704</v>
       </c>
       <c r="C31" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="2">
-        <f t="shared" si="17"/>
-        <v>42704</v>
-      </c>
-      <c r="C32" s="2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update site for cm003 content
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -131,9 +131,6 @@
     <t>Programming in R</t>
   </si>
   <si>
-    <t>Exploratory data analysis</t>
-  </si>
-  <si>
     <t>Introduction to Python</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>Visualizations and the grammar of graphics</t>
+  </si>
+  <si>
+    <t>Data transformation and exploratory data analysis</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,7 +557,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -584,10 +584,10 @@
         <v>42646</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -662,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -692,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -782,7 +782,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -847,7 +847,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="2">
         <v>42641</v>
@@ -856,12 +856,12 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2">
         <f>B22+7</f>
@@ -871,12 +871,12 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" ref="B24:B31" si="17">B23+7</f>
@@ -886,12 +886,12 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="17"/>
@@ -901,12 +901,12 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="17"/>
@@ -916,12 +916,12 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="17"/>
@@ -933,7 +933,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="17"/>
@@ -943,12 +943,12 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="17"/>
@@ -960,7 +960,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="17"/>
@@ -972,7 +972,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="17"/>

</xml_diff>

<commit_message>
Add lab06 materials. Rename files to avoid error rendering site (cannot name multiple files starting with `lab06`)
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>topic</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>More introduction to Python</t>
+  </si>
+  <si>
+    <t>Webdata in Python</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,7 +934,10 @@
         <v>42676</v>
       </c>
       <c r="C27" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add cm012 - web scraping
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="460" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="29960" yWindow="460" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -529,7 +529,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,7 +725,7 @@
         <v>42676</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Switch text and network analysis
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -529,7 +529,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Change content for cm013 and cm014 - both on text analysis
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>topic</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Data wrangling</t>
-  </si>
-  <si>
-    <t>Network analysis</t>
   </si>
   <si>
     <t>Text analysis</t>
@@ -529,7 +526,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,13 +537,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -554,7 +551,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>42639</v>
@@ -563,12 +560,12 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
@@ -578,12 +575,12 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
@@ -593,12 +590,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
@@ -613,7 +610,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
@@ -623,12 +620,12 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
@@ -638,12 +635,12 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
@@ -653,12 +650,12 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
@@ -668,12 +665,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
@@ -683,12 +680,12 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
@@ -698,12 +695,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
@@ -713,12 +710,12 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
@@ -728,12 +725,12 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
@@ -743,12 +740,12 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
@@ -763,7 +760,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
@@ -773,12 +770,12 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
@@ -788,12 +785,12 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
@@ -803,12 +800,12 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
@@ -818,12 +815,12 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
@@ -833,12 +830,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
@@ -848,12 +845,12 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="2">
         <v>42641</v>
@@ -862,12 +859,12 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2">
         <f>B22+7</f>
@@ -877,12 +874,12 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" ref="B24:B31" si="17">B23+7</f>
@@ -892,12 +889,12 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="17"/>
@@ -907,12 +904,12 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="17"/>
@@ -922,12 +919,12 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="17"/>
@@ -937,12 +934,12 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="17"/>
@@ -952,12 +949,12 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="17"/>
@@ -969,7 +966,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="17"/>
@@ -981,7 +978,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="17"/>

</xml_diff>

<commit_message>
Fix link on syllabus
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -38,9 +38,6 @@
     <t>Data wrangling</t>
   </si>
   <si>
-    <t>Text analysis</t>
-  </si>
-  <si>
     <t>Data warehousing and relational databases</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>Text analysis in Python</t>
+  </si>
+  <si>
+    <t>Machine learning</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,13 +540,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>42639</v>
@@ -563,12 +563,12 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
@@ -578,12 +578,12 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
@@ -593,12 +593,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
@@ -613,7 +613,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
@@ -623,12 +623,12 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
@@ -638,12 +638,12 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
@@ -653,12 +653,12 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
@@ -668,12 +668,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
@@ -683,12 +683,12 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
@@ -698,12 +698,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
@@ -713,12 +713,12 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
@@ -728,12 +728,12 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
@@ -743,12 +743,12 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
@@ -758,12 +758,12 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
@@ -773,12 +773,12 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
@@ -788,12 +788,12 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
@@ -803,12 +803,12 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
@@ -818,12 +818,12 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
@@ -833,12 +833,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
@@ -848,12 +848,12 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2">
         <v>42641</v>
@@ -862,12 +862,12 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2">
         <f>B22+7</f>
@@ -877,12 +877,12 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" ref="B24:B31" si="17">B23+7</f>
@@ -892,12 +892,12 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="17"/>
@@ -907,12 +907,12 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="17"/>
@@ -922,12 +922,12 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="17"/>
@@ -937,12 +937,12 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="17"/>
@@ -952,12 +952,12 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="17"/>
@@ -969,7 +969,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="17"/>
@@ -981,7 +981,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="17"/>

</xml_diff>

<commit_message>
Remove dead links on syllabus
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>topic</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Software setup</t>
   </si>
   <si>
-    <t>Pandas</t>
-  </si>
-  <si>
     <t>lab01</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
   </si>
   <si>
     <t>Reproducibility in research</t>
-  </si>
-  <si>
-    <t>Homework help</t>
   </si>
   <si>
     <t>More introduction to Python</t>
@@ -529,7 +523,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -593,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -638,7 +632,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -653,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -668,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -698,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -743,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -758,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -773,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -853,7 +847,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="2">
         <v>42641</v>
@@ -867,7 +861,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2">
         <f>B22+7</f>
@@ -877,12 +871,12 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" ref="B24:B31" si="17">B23+7</f>
@@ -892,12 +886,12 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="17"/>
@@ -906,13 +900,10 @@
       <c r="C25" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D25" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="17"/>
@@ -921,13 +912,10 @@
       <c r="C26" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D26" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="17"/>
@@ -937,12 +925,12 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="17"/>
@@ -952,12 +940,12 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="17"/>
@@ -969,7 +957,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="17"/>
@@ -981,7 +969,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="17"/>

</xml_diff>

<commit_message>
Fix syllabus for cm016
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -200,10 +200,10 @@
     <t>Text analysis in Python</t>
   </si>
   <si>
+    <t>Statistical learning: resampling and tree-based methods</t>
+  </si>
+  <si>
     <t>Statistical learning: basics and classification problems</t>
-  </si>
-  <si>
-    <t>Statistical learning: resampling and tree based methods</t>
   </si>
   <si>
     <t>Statistical learning in Python</t>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -770,7 +770,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -782,10 +782,10 @@
         <v>42690</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update syllabus lab08 title
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29960" yWindow="460" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="7560" yWindow="460" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
     <t>Statistical learning: basics and classification problems</t>
   </si>
   <si>
-    <t>Statistical learning in Python</t>
+    <t>R Markdown websites (and more!)</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix syllabus for cm019
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -38,9 +38,6 @@
     <t>Data wrangling</t>
   </si>
   <si>
-    <t>Interactivity</t>
-  </si>
-  <si>
     <t>Shiny objects</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>Distributed learning: parallel computing</t>
+  </si>
+  <si>
+    <t>Building Shiny apps</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,13 +537,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>42639</v>
@@ -560,12 +560,12 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
@@ -575,12 +575,12 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
@@ -590,12 +590,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
@@ -610,7 +610,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
@@ -620,12 +620,12 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
@@ -635,12 +635,12 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
@@ -650,12 +650,12 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
@@ -665,12 +665,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
@@ -680,12 +680,12 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
@@ -695,12 +695,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
@@ -710,12 +710,12 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
@@ -725,12 +725,12 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
@@ -740,12 +740,12 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
@@ -755,12 +755,12 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
@@ -770,12 +770,12 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
@@ -785,12 +785,12 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
@@ -800,12 +800,12 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
@@ -815,27 +815,27 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
         <v>42702</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
@@ -845,12 +845,12 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2">
         <v>42641</v>
@@ -859,12 +859,12 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="2">
         <f>B22+7</f>
@@ -874,12 +874,12 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" ref="B24:B31" si="17">B23+7</f>
@@ -889,12 +889,12 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="17"/>
@@ -906,7 +906,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="17"/>
@@ -918,7 +918,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="17"/>
@@ -928,12 +928,12 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="17"/>
@@ -943,12 +943,12 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="17"/>
@@ -958,12 +958,12 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="17"/>
@@ -975,7 +975,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="17"/>

</xml_diff>

<commit_message>
Add and update cm019/020 content
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -38,9 +38,6 @@
     <t>Data wrangling</t>
   </si>
   <si>
-    <t>Shiny objects</t>
-  </si>
-  <si>
     <t>cm</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>Building Shiny apps</t>
+  </si>
+  <si>
+    <t>Building Shiny apps (part II)</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,13 +537,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>42639</v>
@@ -560,12 +560,12 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
@@ -575,12 +575,12 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
@@ -590,12 +590,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
@@ -610,7 +610,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
@@ -620,12 +620,12 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
@@ -635,12 +635,12 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
@@ -650,12 +650,12 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
@@ -665,12 +665,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
@@ -680,12 +680,12 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
@@ -695,12 +695,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
@@ -710,12 +710,12 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
@@ -725,12 +725,12 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
@@ -740,12 +740,12 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
@@ -755,12 +755,12 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
@@ -770,12 +770,12 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
@@ -785,12 +785,12 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
@@ -800,12 +800,12 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
@@ -815,12 +815,12 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
@@ -830,27 +830,27 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
         <v>42704</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2">
         <v>42641</v>
@@ -859,12 +859,12 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2">
         <f>B22+7</f>
@@ -874,12 +874,12 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" ref="B24:B31" si="17">B23+7</f>
@@ -889,12 +889,12 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="17"/>
@@ -906,7 +906,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="17"/>
@@ -918,7 +918,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="17"/>
@@ -928,12 +928,12 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="17"/>
@@ -943,12 +943,12 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="17"/>
@@ -958,12 +958,12 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="17"/>
@@ -975,7 +975,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="17"/>

</xml_diff>

<commit_message>
Change syllabus for new term
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>topic</t>
   </si>
@@ -95,18 +95,9 @@
     <t>cm018</t>
   </si>
   <si>
-    <t>cm019</t>
-  </si>
-  <si>
-    <t>cm020</t>
-  </si>
-  <si>
     <t>link_it</t>
   </si>
   <si>
-    <t>Introduction to Python</t>
-  </si>
-  <si>
     <t>Introduction to computing for the social sciences</t>
   </si>
   <si>
@@ -155,58 +146,46 @@
     <t>Data transformation and exploratory data analysis</t>
   </si>
   <si>
-    <t>R Markdown, git, and stuff</t>
-  </si>
-  <si>
     <t>Pipes and functions in R</t>
   </si>
   <si>
-    <t>Using Git in Bash</t>
-  </si>
-  <si>
     <t>Vectors and iteration</t>
   </si>
   <si>
-    <t>Model building</t>
-  </si>
-  <si>
     <t>Reproducibility in research</t>
   </si>
   <si>
-    <t>More introduction to Python</t>
-  </si>
-  <si>
-    <t>Webdata in Python</t>
-  </si>
-  <si>
     <t>Text analysis: fundamentals and sentiment analysis</t>
   </si>
   <si>
     <t>Text analysis: topic modeling</t>
   </si>
   <si>
-    <t>Text analysis in Python</t>
-  </si>
-  <si>
-    <t>Statistical learning: resampling and tree-based methods</t>
-  </si>
-  <si>
-    <t>Statistical learning: basics and classification problems</t>
-  </si>
-  <si>
-    <t>R Markdown websites (and more!)</t>
-  </si>
-  <si>
-    <t>Distributed learning: relational data</t>
-  </si>
-  <si>
-    <t>Distributed learning: parallel computing</t>
-  </si>
-  <si>
     <t>Building Shiny apps</t>
   </si>
   <si>
     <t>Building Shiny apps (part II)</t>
+  </si>
+  <si>
+    <t>No class (MLK Jr. Day)</t>
+  </si>
+  <si>
+    <t>Debugging errors</t>
+  </si>
+  <si>
+    <t>Statistical learning: regression</t>
+  </si>
+  <si>
+    <t>Statistical learning: classification</t>
+  </si>
+  <si>
+    <t>Statistical learning: cross-validation</t>
+  </si>
+  <si>
+    <t>Distributed computing</t>
+  </si>
+  <si>
+    <t>cm000</t>
   </si>
 </sst>
 </file>
@@ -523,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -554,13 +533,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>42639</v>
+        <v>42739</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -568,14 +547,14 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <f>B2+2</f>
-        <v>42641</v>
+        <f>B2+5</f>
+        <v>42744</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -584,82 +563,82 @@
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
-        <v>42646</v>
+        <v>42746</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ref="B5" si="0">B4+2</f>
-        <v>42648</v>
+        <f t="shared" ref="B5:B21" si="0">B4+5</f>
+        <v>42751</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
-        <v>42653</v>
+        <v>42753</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" ref="B7" si="2">B6+2</f>
-        <v>42655</v>
+        <f t="shared" ref="B7:B21" si="2">B6+5</f>
+        <v>42758</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
-        <v>42660</v>
+        <v>42760</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" ref="B9" si="4">B8+2</f>
-        <v>42662</v>
+        <f t="shared" ref="B9:B21" si="4">B8+5</f>
+        <v>42765</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>1</v>
@@ -670,26 +649,26 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
-        <v>42667</v>
+        <v>42767</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" ref="B11" si="6">B10+2</f>
-        <v>42669</v>
+        <f t="shared" ref="B11:B21" si="6">B10+5</f>
+        <v>42772</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>
@@ -700,205 +679,195 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
-        <v>42674</v>
+        <v>42774</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" ref="B13" si="8">B12+2</f>
-        <v>42676</v>
+        <f t="shared" ref="B13:B21" si="8">B12+5</f>
+        <v>42779</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
-        <v>42681</v>
+        <v>42781</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" ref="B15" si="10">B14+2</f>
-        <v>42683</v>
+        <f t="shared" ref="B15:B21" si="10">B14+5</f>
+        <v>42786</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
-        <v>42688</v>
+        <v>42788</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" ref="B17" si="12">B16+2</f>
-        <v>42690</v>
+        <f t="shared" ref="B17:B21" si="12">B16+5</f>
+        <v>42793</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
-        <v>42695</v>
+        <v>42795</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ref="B19" si="14">B18+2</f>
-        <v>42697</v>
+        <f t="shared" ref="B19:B21" si="14">B18+5</f>
+        <v>42800</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
-        <v>42702</v>
+        <v>42802</v>
       </c>
       <c r="C20" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" ref="B21" si="16">B20+2</f>
-        <v>42704</v>
+        <v>42739</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2">
-        <v>42641</v>
+        <v>42744</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2">
-        <f>B22+7</f>
-        <v>42648</v>
+        <f t="shared" ref="B23:B30" si="16">B22+7</f>
+        <v>42751</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2">
-        <f t="shared" ref="B24:B31" si="17">B23+7</f>
-        <v>42655</v>
+        <f t="shared" si="16"/>
+        <v>42758</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" si="17"/>
-        <v>42662</v>
+        <f t="shared" si="16"/>
+        <v>42765</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>0</v>
@@ -906,11 +875,11 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" s="2">
-        <f t="shared" si="17"/>
-        <v>42669</v>
+        <f t="shared" si="16"/>
+        <v>42772</v>
       </c>
       <c r="C26" s="2" t="b">
         <v>0</v>
@@ -918,70 +887,49 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2">
-        <f t="shared" si="17"/>
-        <v>42676</v>
+        <f t="shared" si="16"/>
+        <v>42779</v>
       </c>
       <c r="C27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2">
-        <f t="shared" si="17"/>
-        <v>42683</v>
+        <f t="shared" si="16"/>
+        <v>42786</v>
       </c>
       <c r="C28" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2">
-        <f t="shared" si="17"/>
-        <v>42690</v>
+        <f t="shared" si="16"/>
+        <v>42793</v>
       </c>
       <c r="C29" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="2">
-        <f t="shared" si="17"/>
-        <v>42697</v>
+        <f t="shared" si="16"/>
+        <v>42800</v>
       </c>
       <c r="C30" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="2">
-        <f t="shared" si="17"/>
-        <v>42704</v>
-      </c>
-      <c r="C31" s="2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish updating course objectives - close issue #5
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29960" yWindow="460" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="7560" yWindow="460" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>Text analysis: fundamentals and sentiment analysis</t>
   </si>
   <si>
-    <t>Text analysis: topic modeling</t>
-  </si>
-  <si>
     <t>Building Shiny apps</t>
   </si>
   <si>
@@ -179,13 +176,16 @@
     <t>Statistical learning: classification</t>
   </si>
   <si>
-    <t>Statistical learning: cross-validation</t>
-  </si>
-  <si>
     <t>Distributed computing</t>
   </si>
   <si>
     <t>cm000</t>
+  </si>
+  <si>
+    <t>Statistical learning: resampling methods</t>
+  </si>
+  <si>
+    <t>Text analysis: classification and topic modeling</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -574,17 +574,17 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ref="B5:B21" si="0">B4+5</f>
+        <f t="shared" ref="B5" si="0">B4+5</f>
         <v>42751</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -607,7 +607,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" ref="B7:B21" si="2">B6+5</f>
+        <f t="shared" ref="B7" si="2">B6+5</f>
         <v>42758</v>
       </c>
       <c r="C7" s="2" t="b">
@@ -637,14 +637,14 @@
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" ref="B9:B21" si="4">B8+5</f>
+        <f t="shared" ref="B9" si="4">B8+5</f>
         <v>42765</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -667,14 +667,14 @@
         <v>12</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" ref="B11:B21" si="6">B10+5</f>
+        <f t="shared" ref="B11" si="6">B10+5</f>
         <v>42772</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -697,14 +697,14 @@
         <v>14</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" ref="B13:B21" si="8">B12+5</f>
+        <f t="shared" ref="B13" si="8">B12+5</f>
         <v>42779</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -719,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -727,7 +727,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" ref="B15:B21" si="10">B14+5</f>
+        <f t="shared" ref="B15" si="10">B14+5</f>
         <v>42786</v>
       </c>
       <c r="C15" s="2" t="b">
@@ -757,7 +757,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" ref="B17:B21" si="12">B16+5</f>
+        <f t="shared" ref="B17" si="12">B16+5</f>
         <v>42793</v>
       </c>
       <c r="C17" s="2" t="b">
@@ -779,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -787,14 +787,14 @@
         <v>20</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ref="B19:B21" si="14">B18+5</f>
+        <f t="shared" ref="B19" si="14">B18+5</f>
         <v>42800</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -809,7 +809,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Syllabus - hide future modules and add warning about homework assignments
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -505,7 +505,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,7 +551,7 @@
         <v>42744</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>37</v>
@@ -566,7 +566,7 @@
         <v>42746</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>38</v>
@@ -596,7 +596,7 @@
         <v>42753</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
@@ -611,7 +611,7 @@
         <v>42758</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -626,7 +626,7 @@
         <v>42760</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
@@ -641,7 +641,7 @@
         <v>42765</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -656,7 +656,7 @@
         <v>42767</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>41</v>
@@ -671,7 +671,7 @@
         <v>42772</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -686,7 +686,7 @@
         <v>42774</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>48</v>
@@ -701,7 +701,7 @@
         <v>42779</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>51</v>
@@ -716,7 +716,7 @@
         <v>42781</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>49</v>
@@ -731,7 +731,7 @@
         <v>42786</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>
@@ -746,7 +746,7 @@
         <v>42788</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
@@ -761,7 +761,7 @@
         <v>42793</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>42</v>
@@ -776,7 +776,7 @@
         <v>42795</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>52</v>
@@ -791,7 +791,7 @@
         <v>42800</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>43</v>
@@ -806,7 +806,7 @@
         <v>42802</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Render site with lab01 and lab02
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>topic</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Text analysis: classification and topic modeling</t>
+  </si>
+  <si>
+    <t>R basics</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,7 +554,7 @@
         <v>42744</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>37</v>
@@ -820,7 +823,7 @@
         <v>42739</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
         <v>26</v>
@@ -834,7 +837,10 @@
         <v>42744</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update instructions and schedule for cm002-4
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -508,7 +508,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,7 +569,7 @@
         <v>42746</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Add cm005 to syllabus
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,7 +617,7 @@
         <v>42758</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -877,7 +877,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" ref="B23:B30" si="16">B24+7</f>
+        <f t="shared" ref="B25:B30" si="16">B24+7</f>
         <v>42765</v>
       </c>
       <c r="C25" s="2" t="b">

</xml_diff>

<commit_message>
Render site for cm006
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,7 +632,7 @@
         <v>42760</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Add cm007 to syllabus
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -167,9 +167,6 @@
     <t>No class (MLK Jr. Day)</t>
   </si>
   <si>
-    <t>Debugging errors</t>
-  </si>
-  <si>
     <t>Statistical learning: regression</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>Graphing tips for `ggplot2` (and life)</t>
+  </si>
+  <si>
+    <t>Debugging and defensive programming</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,7 +580,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+5</f>
@@ -647,10 +647,10 @@
         <v>42765</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -680,7 +680,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -843,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -857,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update cm008 and add to syllabus
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -152,9 +152,6 @@
     <t>Vectors and iteration</t>
   </si>
   <si>
-    <t>Reproducibility in research</t>
-  </si>
-  <si>
     <t>Text analysis: fundamentals and sentiment analysis</t>
   </si>
   <si>
@@ -167,9 +164,6 @@
     <t>No class (MLK Jr. Day)</t>
   </si>
   <si>
-    <t>Statistical learning: regression</t>
-  </si>
-  <si>
     <t>Statistical learning: classification</t>
   </si>
   <si>
@@ -192,6 +186,12 @@
   </si>
   <si>
     <t>Debugging and defensive programming</t>
+  </si>
+  <si>
+    <t>A deep dive into R Markdown</t>
+  </si>
+  <si>
+    <t>Statistical learning: basics and linear regression</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,7 +580,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+5</f>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -650,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -662,10 +662,10 @@
         <v>42767</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -680,7 +680,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -695,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -843,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -857,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Render site for cm009
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,7 +677,7 @@
         <v>42772</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Update cm010 and add to syllabus
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,7 +692,7 @@
         <v>42774</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Render site for cm012 and hw07
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -167,9 +167,6 @@
     <t>Statistical learning: classification</t>
   </si>
   <si>
-    <t>Distributed computing</t>
-  </si>
-  <si>
     <t>cm000</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>Statistical learning: basics and linear regression</t>
+  </si>
+  <si>
+    <t>Distributed learning</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,7 +580,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+5</f>
@@ -650,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -665,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -680,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -722,10 +722,10 @@
         <v>42781</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -843,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -857,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Publish cm013 and render site
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,7 +737,7 @@
         <v>42786</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Update and publish cm014
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,7 +752,7 @@
         <v>42788</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Add cm015 to syllabus
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,7 +767,7 @@
         <v>42793</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Add cm016 and hw09 to syllabus and update site
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,7 +782,7 @@
         <v>42795</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Add cm017 and cm018 to syllabus
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -511,7 +511,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -797,7 +797,7 @@
         <v>42800</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>42</v>
@@ -812,7 +812,7 @@
         <v>42802</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update schedule for fall 2017
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="460" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="1700" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>topic</t>
   </si>
@@ -143,33 +143,15 @@
     <t>Visualizations and the grammar of graphics</t>
   </si>
   <si>
-    <t>Data transformation and exploratory data analysis</t>
-  </si>
-  <si>
-    <t>Pipes and functions in R</t>
-  </si>
-  <si>
     <t>Vectors and iteration</t>
   </si>
   <si>
     <t>Text analysis: fundamentals and sentiment analysis</t>
   </si>
   <si>
-    <t>Building Shiny apps</t>
-  </si>
-  <si>
-    <t>Building Shiny apps (part II)</t>
-  </si>
-  <si>
-    <t>No class (MLK Jr. Day)</t>
-  </si>
-  <si>
     <t>Statistical learning: classification</t>
   </si>
   <si>
-    <t>cm000</t>
-  </si>
-  <si>
     <t>Statistical learning: resampling methods</t>
   </si>
   <si>
@@ -185,13 +167,43 @@
     <t>Debugging and defensive programming</t>
   </si>
   <si>
-    <t>A deep dive into R Markdown</t>
-  </si>
-  <si>
     <t>Statistical learning: basics and linear regression</t>
   </si>
   <si>
     <t>Distributed learning</t>
+  </si>
+  <si>
+    <t>cm019</t>
+  </si>
+  <si>
+    <t>cm020</t>
+  </si>
+  <si>
+    <t>Data transformation</t>
+  </si>
+  <si>
+    <t>Exploratory data analysis</t>
+  </si>
+  <si>
+    <t>Data wrangling (more)</t>
+  </si>
+  <si>
+    <t>Shiny applications</t>
+  </si>
+  <si>
+    <t>Interactivity in R</t>
+  </si>
+  <si>
+    <t>Pipes and functions</t>
+  </si>
+  <si>
+    <t>R Markdown</t>
+  </si>
+  <si>
+    <t>The shell</t>
+  </si>
+  <si>
+    <t>AWS</t>
   </si>
 </sst>
 </file>
@@ -508,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -539,7 +551,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>42739</v>
+        <v>43003</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -553,8 +565,8 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <f>B2+5</f>
-        <v>42744</v>
+        <f>B2+2</f>
+        <v>43005</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -569,37 +581,37 @@
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
-        <v>42746</v>
+        <v>43010</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ref="B5" si="0">B4+5</f>
-        <v>42751</v>
+        <f t="shared" ref="B5" si="0">B4+2</f>
+        <v>43012</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
-        <v>42753</v>
+        <v>43017</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -610,191 +622,191 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" ref="B7" si="2">B6+5</f>
-        <v>42758</v>
+        <f t="shared" ref="B7" si="2">B6+2</f>
+        <v>43019</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
-        <v>42760</v>
+        <v>43024</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" ref="B9" si="4">B8+5</f>
-        <v>42765</v>
+        <f t="shared" ref="B9" si="4">B8+2</f>
+        <v>43026</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
-        <v>42767</v>
+        <v>43031</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" ref="B11" si="6">B10+5</f>
-        <v>42772</v>
+        <f t="shared" ref="B11" si="6">B10+2</f>
+        <v>43033</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
-        <v>42774</v>
+        <v>43038</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" ref="B13" si="8">B12+5</f>
-        <v>42779</v>
+        <f t="shared" ref="B13" si="8">B12+2</f>
+        <v>43040</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
-        <v>42781</v>
+        <v>43045</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" ref="B15" si="10">B14+5</f>
-        <v>42786</v>
+        <f t="shared" ref="B15" si="10">B14+2</f>
+        <v>43047</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
-        <v>42788</v>
+        <v>43052</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" ref="B17" si="12">B16+5</f>
-        <v>42793</v>
+        <f t="shared" ref="B17" si="12">B16+2</f>
+        <v>43054</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
-        <v>42795</v>
+        <v>43059</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ref="B19" si="14">B18+5</f>
-        <v>42800</v>
+        <f t="shared" ref="B19" si="14">B18+2</f>
+        <v>43061</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>1</v>
@@ -805,92 +817,100 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
-        <v>42802</v>
+        <v>43066</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="B21" s="2">
-        <v>42739</v>
+        <f t="shared" ref="B21" si="16">B20+2</f>
+        <v>43068</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2">
-        <v>42744</v>
+        <v>43005</v>
       </c>
       <c r="C22" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2">
-        <v>42753</v>
+        <f>B22+7</f>
+        <v>43012</v>
       </c>
       <c r="C23" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2">
-        <f>B22+14</f>
-        <v>42758</v>
+        <f t="shared" ref="B24:B31" si="17">B23+7</f>
+        <v>43019</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" ref="B25:B30" si="16">B24+7</f>
-        <v>42765</v>
+        <f t="shared" si="17"/>
+        <v>43026</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2">
-        <f t="shared" si="16"/>
-        <v>42772</v>
+        <f t="shared" si="17"/>
+        <v>43033</v>
       </c>
       <c r="C26" s="2" t="b">
         <v>0</v>
@@ -898,11 +918,11 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2">
-        <f t="shared" si="16"/>
-        <v>42779</v>
+        <f t="shared" si="17"/>
+        <v>43040</v>
       </c>
       <c r="C27" s="2" t="b">
         <v>0</v>
@@ -910,23 +930,26 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2">
-        <f t="shared" si="16"/>
-        <v>42786</v>
+        <f t="shared" si="17"/>
+        <v>43047</v>
       </c>
       <c r="C28" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2">
-        <f t="shared" si="16"/>
-        <v>42793</v>
+        <f t="shared" si="17"/>
+        <v>43054</v>
       </c>
       <c r="C29" s="2" t="b">
         <v>0</v>
@@ -934,13 +957,25 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2">
+        <f t="shared" si="17"/>
+        <v>43061</v>
+      </c>
+      <c r="C30" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="2">
-        <f t="shared" si="16"/>
-        <v>42800</v>
-      </c>
-      <c r="C30" s="2" t="b">
+      <c r="B31" s="2">
+        <f t="shared" si="17"/>
+        <v>43068</v>
+      </c>
+      <c r="C31" s="2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Organize data wrangling lessons
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -35,9 +35,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>Data wrangling</t>
-  </si>
-  <si>
     <t>cm</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>Exploratory data analysis</t>
   </si>
   <si>
-    <t>Data wrangling (more)</t>
-  </si>
-  <si>
     <t>Shiny applications</t>
   </si>
   <si>
@@ -204,6 +198,12 @@
   </si>
   <si>
     <t>AWS</t>
+  </si>
+  <si>
+    <t>Data wrangling: tidy data</t>
+  </si>
+  <si>
+    <t>Data wrangling: relational data and factors</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,13 +534,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>43003</v>
@@ -557,12 +557,12 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
@@ -572,12 +572,12 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
@@ -587,12 +587,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
@@ -602,12 +602,12 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
@@ -617,12 +617,12 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
@@ -632,12 +632,12 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
@@ -647,12 +647,12 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
@@ -662,12 +662,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
@@ -677,12 +677,12 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
@@ -692,12 +692,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
@@ -707,12 +707,12 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
@@ -722,12 +722,12 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
@@ -737,12 +737,12 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
@@ -752,12 +752,12 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
@@ -767,12 +767,12 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
@@ -782,12 +782,12 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
@@ -797,12 +797,12 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
@@ -812,12 +812,12 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
@@ -827,12 +827,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
@@ -842,12 +842,12 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2">
         <v>43005</v>
@@ -856,12 +856,12 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2">
         <f>B22+7</f>
@@ -871,12 +871,12 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" ref="B24:B31" si="17">B23+7</f>
@@ -886,12 +886,12 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="17"/>
@@ -901,12 +901,12 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" si="17"/>
@@ -918,7 +918,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2">
         <f t="shared" si="17"/>
@@ -930,7 +930,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" si="17"/>
@@ -940,12 +940,12 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2">
         <f t="shared" si="17"/>
@@ -957,7 +957,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="17"/>
@@ -969,7 +969,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="17"/>

</xml_diff>

<commit_message>
Remove lab03 from schedule temporarily
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="440" yWindow="1700" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="780" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,7 +883,7 @@
         <v>43019</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Remove lab modules that don't exist
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>topic</t>
   </si>
@@ -158,9 +158,6 @@
     <t>R basics</t>
   </si>
   <si>
-    <t>Graphing tips for `ggplot2` (and life)</t>
-  </si>
-  <si>
     <t>Debugging and defensive programming</t>
   </si>
   <si>
@@ -192,12 +189,6 @@
   </si>
   <si>
     <t>R Markdown</t>
-  </si>
-  <si>
-    <t>The shell</t>
-  </si>
-  <si>
-    <t>AWS</t>
   </si>
   <si>
     <t>Data wrangling: tidy data</t>
@@ -523,7 +514,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D24" sqref="D24:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -602,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -617,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -632,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -647,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -692,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -707,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -752,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -817,7 +808,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
@@ -827,12 +818,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
@@ -842,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -885,9 +876,6 @@
       <c r="C24" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D24" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -900,9 +888,6 @@
       <c r="C25" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D25" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -938,9 +923,6 @@
       </c>
       <c r="C28" s="2" t="b">
         <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add geospatial viz to cm014, compress stat learning to 1 week
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -146,12 +146,6 @@
     <t>Text analysis: fundamentals and sentiment analysis</t>
   </si>
   <si>
-    <t>Statistical learning: classification</t>
-  </si>
-  <si>
-    <t>Statistical learning: resampling methods</t>
-  </si>
-  <si>
     <t>Text analysis: classification and topic modeling</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>Debugging and defensive programming</t>
   </si>
   <si>
-    <t>Statistical learning: basics and linear regression</t>
-  </si>
-  <si>
     <t>Distributed learning</t>
   </si>
   <si>
@@ -195,6 +186,15 @@
   </si>
   <si>
     <t>Data wrangling: relational data and factors</t>
+  </si>
+  <si>
+    <t>Geospatial visualization</t>
+  </si>
+  <si>
+    <t>Statistical learning: regression and classification</t>
+  </si>
+  <si>
+    <t>Statistical learning: classification and cross-validation</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D28"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -608,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -638,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -668,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -698,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -728,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -743,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -803,12 +803,12 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
@@ -818,12 +818,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
@@ -833,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -862,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update syllabus for a full Shiny week
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -170,12 +170,6 @@
     <t>Exploratory data analysis</t>
   </si>
   <si>
-    <t>Shiny applications</t>
-  </si>
-  <si>
-    <t>Interactivity in R</t>
-  </si>
-  <si>
     <t>Pipes and functions</t>
   </si>
   <si>
@@ -195,6 +189,12 @@
   </si>
   <si>
     <t>Statistical learning: classification and cross-validation</t>
+  </si>
+  <si>
+    <t>Building Shiny applications</t>
+  </si>
+  <si>
+    <t>Building Shiny applications (part II)</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -638,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -698,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -743,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -815,10 +815,10 @@
         <v>43066</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -833,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Convert syllabus to spring 2018 dates
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="440" yWindow="780" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -194,13 +194,13 @@
     <t>Building Shiny applications</t>
   </si>
   <si>
-    <t>Building Shiny applications (part II)</t>
+    <t>Memorial day (no class)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -243,6 +243,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -514,7 +517,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>43003</v>
+        <v>43185</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -557,7 +560,7 @@
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
-        <v>43005</v>
+        <v>43187</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -572,7 +575,7 @@
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
-        <v>43010</v>
+        <v>43192</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -587,7 +590,7 @@
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
-        <v>43012</v>
+        <v>43194</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -602,7 +605,7 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
-        <v>43017</v>
+        <v>43199</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -617,7 +620,7 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
-        <v>43019</v>
+        <v>43201</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -632,7 +635,7 @@
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
-        <v>43024</v>
+        <v>43206</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>1</v>
@@ -647,7 +650,7 @@
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
-        <v>43026</v>
+        <v>43208</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>1</v>
@@ -662,7 +665,7 @@
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
-        <v>43031</v>
+        <v>43213</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>1</v>
@@ -677,7 +680,7 @@
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
-        <v>43033</v>
+        <v>43215</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>
@@ -692,7 +695,7 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
-        <v>43038</v>
+        <v>43220</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>1</v>
@@ -707,7 +710,7 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
-        <v>43040</v>
+        <v>43222</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
@@ -722,7 +725,7 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
-        <v>43045</v>
+        <v>43227</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>1</v>
@@ -737,7 +740,7 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
-        <v>43047</v>
+        <v>43229</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>1</v>
@@ -752,7 +755,7 @@
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
-        <v>43052</v>
+        <v>43234</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>1</v>
@@ -767,7 +770,7 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
-        <v>43054</v>
+        <v>43236</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>1</v>
@@ -782,7 +785,7 @@
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
-        <v>43059</v>
+        <v>43241</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>1</v>
@@ -797,7 +800,7 @@
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
-        <v>43061</v>
+        <v>43243</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>1</v>
@@ -812,13 +815,13 @@
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
-        <v>43066</v>
+        <v>43248</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -827,13 +830,13 @@
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
-        <v>43068</v>
+        <v>43250</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -841,7 +844,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="2">
-        <v>43005</v>
+        <v>43187</v>
       </c>
       <c r="C22" s="2" t="b">
         <v>1</v>
@@ -856,7 +859,7 @@
       </c>
       <c r="B23" s="2">
         <f>B22+7</f>
-        <v>43012</v>
+        <v>43194</v>
       </c>
       <c r="C23" s="2" t="b">
         <v>1</v>
@@ -871,7 +874,7 @@
       </c>
       <c r="B24" s="2">
         <f t="shared" ref="B24:B31" si="17">B23+7</f>
-        <v>43019</v>
+        <v>43201</v>
       </c>
       <c r="C24" s="2" t="b">
         <v>0</v>
@@ -883,7 +886,7 @@
       </c>
       <c r="B25" s="2">
         <f t="shared" si="17"/>
-        <v>43026</v>
+        <v>43208</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>0</v>
@@ -895,7 +898,7 @@
       </c>
       <c r="B26" s="2">
         <f t="shared" si="17"/>
-        <v>43033</v>
+        <v>43215</v>
       </c>
       <c r="C26" s="2" t="b">
         <v>0</v>
@@ -907,7 +910,7 @@
       </c>
       <c r="B27" s="2">
         <f t="shared" si="17"/>
-        <v>43040</v>
+        <v>43222</v>
       </c>
       <c r="C27" s="2" t="b">
         <v>0</v>
@@ -919,7 +922,7 @@
       </c>
       <c r="B28" s="2">
         <f t="shared" si="17"/>
-        <v>43047</v>
+        <v>43229</v>
       </c>
       <c r="C28" s="2" t="b">
         <v>0</v>
@@ -931,7 +934,7 @@
       </c>
       <c r="B29" s="2">
         <f t="shared" si="17"/>
-        <v>43054</v>
+        <v>43236</v>
       </c>
       <c r="C29" s="2" t="b">
         <v>0</v>
@@ -943,7 +946,7 @@
       </c>
       <c r="B30" s="2">
         <f t="shared" si="17"/>
-        <v>43061</v>
+        <v>43243</v>
       </c>
       <c r="C30" s="2" t="b">
         <v>0</v>
@@ -955,7 +958,7 @@
       </c>
       <c r="B31" s="2">
         <f t="shared" si="17"/>
-        <v>43068</v>
+        <v>43250</v>
       </c>
       <c r="C31" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Update syllabus dates and remove labs from the syllabus - we don't do anything formal during those sessions.
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Computing for Social Sciences/uc-cfss.github.io/course_admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E13DC14-828D-D145-A012-67E56CCCD44F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>topic</t>
   </si>
@@ -104,39 +105,6 @@
     <t>Getting data from the web: scraping</t>
   </si>
   <si>
-    <t>Software setup</t>
-  </si>
-  <si>
-    <t>lab01</t>
-  </si>
-  <si>
-    <t>lab02</t>
-  </si>
-  <si>
-    <t>lab03</t>
-  </si>
-  <si>
-    <t>lab04</t>
-  </si>
-  <si>
-    <t>lab05</t>
-  </si>
-  <si>
-    <t>lab06</t>
-  </si>
-  <si>
-    <t>lab07</t>
-  </si>
-  <si>
-    <t>lab08</t>
-  </si>
-  <si>
-    <t>lab09</t>
-  </si>
-  <si>
-    <t>lab10</t>
-  </si>
-  <si>
     <t>Visualizations and the grammar of graphics</t>
   </si>
   <si>
@@ -149,9 +117,6 @@
     <t>Text analysis: classification and topic modeling</t>
   </si>
   <si>
-    <t>R basics</t>
-  </si>
-  <si>
     <t>Debugging and defensive programming</t>
   </si>
   <si>
@@ -194,13 +159,13 @@
     <t>Building Shiny applications</t>
   </si>
   <si>
-    <t>Memorial day (no class)</t>
+    <t>Building Shiny applications (part II)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -513,11 +478,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,7 +510,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>43185</v>
+        <v>43374</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -560,13 +525,13 @@
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
-        <v>43187</v>
+        <v>43376</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -575,13 +540,13 @@
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
-        <v>43192</v>
+        <v>43381</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -590,13 +555,13 @@
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
-        <v>43194</v>
+        <v>43383</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -605,13 +570,13 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
-        <v>43199</v>
+        <v>43388</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -620,13 +585,13 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
-        <v>43201</v>
+        <v>43390</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -635,13 +600,13 @@
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
-        <v>43206</v>
+        <v>43395</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -650,13 +615,13 @@
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
-        <v>43208</v>
+        <v>43397</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -665,13 +630,13 @@
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
-        <v>43213</v>
+        <v>43402</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -680,13 +645,13 @@
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
-        <v>43215</v>
+        <v>43404</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -695,13 +660,13 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
-        <v>43220</v>
+        <v>43409</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -710,13 +675,13 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
-        <v>43222</v>
+        <v>43411</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -725,13 +690,13 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
-        <v>43227</v>
+        <v>43416</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -740,13 +705,13 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
-        <v>43229</v>
+        <v>43418</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -755,7 +720,7 @@
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
-        <v>43234</v>
+        <v>43423</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>1</v>
@@ -770,7 +735,7 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
-        <v>43236</v>
+        <v>43425</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>1</v>
@@ -785,13 +750,13 @@
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
-        <v>43241</v>
+        <v>43430</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -800,168 +765,43 @@
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
-        <v>43243</v>
+        <v>43432</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
-        <v>43248</v>
+        <v>43437</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
-        <v>43250</v>
+        <v>43439</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="2">
-        <v>43187</v>
-      </c>
-      <c r="C22" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="2">
-        <f>B22+7</f>
-        <v>43194</v>
-      </c>
-      <c r="C23" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="2">
-        <f t="shared" ref="B24:B31" si="17">B23+7</f>
-        <v>43201</v>
-      </c>
-      <c r="C24" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="2">
-        <f t="shared" si="17"/>
-        <v>43208</v>
-      </c>
-      <c r="C25" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="2">
-        <f t="shared" si="17"/>
-        <v>43215</v>
-      </c>
-      <c r="C26" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="2">
-        <f t="shared" si="17"/>
-        <v>43222</v>
-      </c>
-      <c r="C27" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="2">
-        <f t="shared" si="17"/>
-        <v>43229</v>
-      </c>
-      <c r="C28" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="2">
-        <f t="shared" si="17"/>
-        <v>43236</v>
-      </c>
-      <c r="C29" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="2">
-        <f t="shared" si="17"/>
-        <v>43243</v>
-      </c>
-      <c r="C30" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="2">
-        <f t="shared" si="17"/>
-        <v>43250</v>
-      </c>
-      <c r="C31" s="2" t="b">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retitle cm019 and cm020
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Computing for Social Sciences/uc-cfss.github.io/course_admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E13DC14-828D-D145-A012-67E56CCCD44F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D7FE0C-81B3-DC44-B27C-C8AB74BF2A35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,10 +156,10 @@
     <t>Statistical learning: classification and cross-validation</t>
   </si>
   <si>
-    <t>Building Shiny applications</t>
-  </si>
-  <si>
-    <t>Building Shiny applications (part II)</t>
+    <t>Building Shiny applications: user interface</t>
+  </si>
+  <si>
+    <t>Building Shiny applications: server</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Update syllabus for spring 19
</commit_message>
<xml_diff>
--- a/course_admin/schedule.xlsx
+++ b/course_admin/schedule.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Computing for Social Sciences/uc-cfss.github.io/course_admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D7FE0C-81B3-DC44-B27C-C8AB74BF2A35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FE5293-C749-C540-AB2B-49852BCB4588}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,7 +510,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>43374</v>
+        <v>43556</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -525,7 +525,7 @@
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
-        <v>43376</v>
+        <v>43558</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -540,7 +540,7 @@
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
-        <v>43381</v>
+        <v>43563</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -555,7 +555,7 @@
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
-        <v>43383</v>
+        <v>43565</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -570,7 +570,7 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
-        <v>43388</v>
+        <v>43570</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -585,7 +585,7 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
-        <v>43390</v>
+        <v>43572</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -600,7 +600,7 @@
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
-        <v>43395</v>
+        <v>43577</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>1</v>
@@ -615,7 +615,7 @@
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
-        <v>43397</v>
+        <v>43579</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>1</v>
@@ -630,7 +630,7 @@
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
-        <v>43402</v>
+        <v>43584</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>1</v>
@@ -645,7 +645,7 @@
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
-        <v>43404</v>
+        <v>43586</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>
@@ -660,7 +660,7 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
-        <v>43409</v>
+        <v>43591</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>1</v>
@@ -675,7 +675,7 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
-        <v>43411</v>
+        <v>43593</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
@@ -690,7 +690,7 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
-        <v>43416</v>
+        <v>43598</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>1</v>
@@ -705,7 +705,7 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
-        <v>43418</v>
+        <v>43600</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>1</v>
@@ -720,7 +720,7 @@
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
-        <v>43423</v>
+        <v>43605</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>1</v>
@@ -735,7 +735,7 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
-        <v>43425</v>
+        <v>43607</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>1</v>
@@ -750,7 +750,7 @@
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
-        <v>43430</v>
+        <v>43612</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>1</v>
@@ -765,7 +765,7 @@
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
-        <v>43432</v>
+        <v>43614</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>1</v>
@@ -780,7 +780,7 @@
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
-        <v>43437</v>
+        <v>43619</v>
       </c>
       <c r="C20" s="2" t="b">
         <v>1</v>
@@ -795,7 +795,7 @@
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
-        <v>43439</v>
+        <v>43621</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>1</v>

</xml_diff>